<commit_message>
Reapply "Add files via upload"
This reverts commit c418b2ae08029730d5cb723fa225cfa7b0e251c6.
</commit_message>
<xml_diff>
--- a/Lean-Projektovy-Management-Prazdna-sablona-JiriBenedikt.com-CZ.xlsx
+++ b/Lean-Projektovy-Management-Prazdna-sablona-JiriBenedikt.com-CZ.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KucharJan\Documents\ProjektPXPR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MachacekDav\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FFD032-6491-46CA-8FD2-28A0B8C74610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D32308-1B69-486B-89E0-44890CAFA37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zakládací listina " sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="132">
   <si>
     <t>Zakládací listina projektu</t>
   </si>
@@ -317,9 +317,6 @@
     <t>Vybrat spolehlivého poskytovatele webhostingu s vysokou dostupností (minimálně 99,9 % uptime).</t>
   </si>
   <si>
-    <t xml:space="preserve">Výběr platformy WordPress	</t>
-  </si>
-  <si>
     <t xml:space="preserve">Zálohování a bezpečnost	</t>
   </si>
   <si>
@@ -362,9 +359,6 @@
     <t>Testování systému, rychlé opravy, zajištění podpory v případě problémů.</t>
   </si>
   <si>
-    <t>Instalace SSL certifikátu, aktualizace WordPressu a pluginů, použití bezpečnostních pluginů.</t>
-  </si>
-  <si>
     <t>Rezervační systém</t>
   </si>
   <si>
@@ -389,9 +383,6 @@
     <t>Internetová stránka s rezervací lístků na maturitní ples</t>
   </si>
   <si>
-    <t>Naším cílem je vytvořit webové stránky pomocí platformy WordPress, které budou sloužit jako oficiální stránka našeho maturitního plesu. Stránky budou obsahovat možnost online rezervace vstupenek, informace o programu plesu, a další potřebné informace pro účastníky.</t>
-  </si>
-  <si>
     <t>Cílem projektu je usnadnit rezervaci vstupenek na náš maturitní ples pomocí uživatelsky přívětivého webového rozhraní. Stránky budou sloužit jako hlavní komunikační kanál pro účastníky, což zajistí pohodlný a rychlý přístup k informacím o akci.</t>
   </si>
   <si>
@@ -401,9 +392,6 @@
     <t>Zkrácení času potřebného pro zpracování rezervací oproti tradičním metodám (např. fyzický prodej), s plánem automatizovat 90 % procesů.</t>
   </si>
   <si>
-    <t xml:space="preserve">Vytvoření webových stránek na platformě WordPress. Implementace systému pro online rezervace vstupenek na maturitní ples. Integrace informací o plesu, programu, místě konání a dalších důležitých detailech. </t>
-  </si>
-  <si>
     <t>Revize funkčnosti webu a návrhy na úpravy  a testování a příprava na spuštění</t>
   </si>
   <si>
@@ -429,6 +417,30 @@
   </si>
   <si>
     <t>Komunikace</t>
+  </si>
+  <si>
+    <t>instalace ENDORY</t>
+  </si>
+  <si>
+    <t>Začátek a spuštění ENDORY</t>
+  </si>
+  <si>
+    <t>Výběr a instalace Endory platformy</t>
+  </si>
+  <si>
+    <t>instalace Endory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vytvoření webových stránek na platformě Endora. Implementace systému pro online rezervace vstupenek na maturitní ples. Integrace informací o plesu, programu, místě konání a dalších důležitých detailech. </t>
+  </si>
+  <si>
+    <t>Instalace SSL certifikátu, aktualizace Endora a pluginů, použití bezpečnostních pluginů.</t>
+  </si>
+  <si>
+    <t>Výběr platformy Endora</t>
+  </si>
+  <si>
+    <t>Naším cílem je vytvořit webové stránky pomocí platformy Endora, které budou sloužit jako oficiální stránka našeho maturitního plesu. Stránky budou obsahovat možnost online rezervace vstupenek, informace o programu plesu, a další potřebné informace pro účastníky.</t>
   </si>
 </sst>
 </file>
@@ -1461,76 +1473,127 @@
     <xf numFmtId="168" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1540,58 +1603,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -2307,8 +2319,8 @@
   </sheetPr>
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2325,13 +2337,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
       <c r="F1" s="64"/>
       <c r="G1" s="64"/>
       <c r="H1" s="64"/>
@@ -2342,28 +2354,28 @@
       <c r="A3" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="106" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="106"/>
+      <c r="B3" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="107"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="107" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="106"/>
+      <c r="C4" s="107"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="107" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="106"/>
+      <c r="C5" s="107"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="55" t="s">
@@ -2412,53 +2424,53 @@
       <c r="A13" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="97" t="s">
-        <v>114</v>
-      </c>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="99"/>
+      <c r="B13" s="98" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="100"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="100"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="102"/>
+      <c r="B14" s="101"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="103"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="100"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="102"/>
+      <c r="B15" s="101"/>
+      <c r="C15" s="102"/>
+      <c r="D15" s="102"/>
+      <c r="E15" s="103"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="103"/>
-      <c r="C16" s="104"/>
-      <c r="D16" s="104"/>
-      <c r="E16" s="105"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="106"/>
     </row>
     <row r="17" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="97" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="99"/>
+      <c r="B17" s="98" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="99"/>
+      <c r="D17" s="99"/>
+      <c r="E17" s="100"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="100"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="102"/>
+      <c r="B18" s="101"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="103"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="103"/>
-      <c r="C19" s="104"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="105"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="106"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="59"/>
@@ -2482,14 +2494,14 @@
     </row>
     <row r="22" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B22" s="56" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C22" s="58"/>
       <c r="D22" s="58"/>
     </row>
     <row r="23" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B23" s="56" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C23" s="58"/>
       <c r="D23" s="58"/>
@@ -2508,45 +2520,45 @@
       <c r="B26" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="94" t="s">
+      <c r="C26" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="94"/>
-      <c r="E26" s="94"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="107" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" s="108" t="s">
+      <c r="B27" s="89" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="108"/>
-      <c r="E27" s="108"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="107"/>
-      <c r="C28" s="108"/>
-      <c r="D28" s="108"/>
-      <c r="E28" s="108"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="90"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="107"/>
-      <c r="C29" s="108"/>
-      <c r="D29" s="108"/>
-      <c r="E29" s="108"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="90"/>
+      <c r="E29" s="90"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="107"/>
-      <c r="C30" s="108"/>
-      <c r="D30" s="108"/>
-      <c r="E30" s="108"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
     </row>
     <row r="31" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="107"/>
-      <c r="C31" s="108"/>
-      <c r="D31" s="108"/>
-      <c r="E31" s="108"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="90"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="90"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="55" t="s">
@@ -2569,7 +2581,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" s="56" t="s">
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="C35" s="63">
         <v>45599</v>
@@ -2585,7 +2597,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="56" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C37" s="63">
         <v>45689</v>
@@ -2606,61 +2618,61 @@
       <c r="B40" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="95" t="s">
+      <c r="C40" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="95"/>
-      <c r="E40" s="95"/>
+      <c r="D40" s="96"/>
+      <c r="E40" s="96"/>
     </row>
     <row r="41" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="90" t="s">
+      <c r="C41" s="91" t="s">
         <v>89</v>
       </c>
-      <c r="D41" s="109"/>
-      <c r="E41" s="91"/>
+      <c r="D41" s="92"/>
+      <c r="E41" s="93"/>
     </row>
     <row r="42" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="90" t="s">
-        <v>101</v>
-      </c>
-      <c r="D42" s="109"/>
-      <c r="E42" s="91"/>
+      <c r="C42" s="91" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="92"/>
+      <c r="E42" s="93"/>
     </row>
     <row r="43" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="90" t="s">
-        <v>102</v>
-      </c>
-      <c r="D43" s="109"/>
-      <c r="E43" s="91"/>
+      <c r="C43" s="91" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" s="92"/>
+      <c r="E43" s="93"/>
     </row>
     <row r="44" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="90" t="s">
-        <v>104</v>
-      </c>
-      <c r="D44" s="109"/>
-      <c r="E44" s="91"/>
+      <c r="D44" s="92"/>
+      <c r="E44" s="93"/>
     </row>
     <row r="45" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="110" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" s="110"/>
-      <c r="E45" s="110"/>
+      <c r="C45" s="94" t="s">
+        <v>129</v>
+      </c>
+      <c r="D45" s="94"/>
+      <c r="E45" s="94"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="55" t="s">
@@ -2672,20 +2684,20 @@
       <c r="C48" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D48" s="95" t="s">
+      <c r="D48" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="E48" s="95"/>
+      <c r="E48" s="96"/>
     </row>
     <row r="49" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="53" t="s">
         <v>45</v>
       </c>
       <c r="B49" s="65" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="C49" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D49" s="88">
         <v>0</v>
@@ -2694,7 +2706,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" s="65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C50" s="56" t="s">
         <v>75</v>
@@ -2706,7 +2718,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" s="56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C51" s="56" t="s">
         <v>80</v>
@@ -2718,7 +2730,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C52" s="56" t="s">
         <v>77</v>
@@ -2730,7 +2742,7 @@
     </row>
     <row r="53" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B53" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C53" s="56" t="s">
         <v>76</v>
@@ -2743,8 +2755,8 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" s="69"/>
       <c r="C54" s="69"/>
-      <c r="D54" s="89"/>
-      <c r="E54" s="89"/>
+      <c r="D54" s="108"/>
+      <c r="E54" s="108"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="55" t="s">
@@ -2762,45 +2774,60 @@
     </row>
     <row r="57" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B57" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="C57" s="68" t="s">
+      <c r="D57" s="91" t="s">
         <v>95</v>
       </c>
-      <c r="D57" s="90" t="s">
-        <v>96</v>
-      </c>
-      <c r="E57" s="91"/>
+      <c r="E57" s="93"/>
     </row>
     <row r="58" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B58" s="67" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C58" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="D58" s="92" t="s">
-        <v>99</v>
-      </c>
-      <c r="E58" s="93"/>
+        <v>94</v>
+      </c>
+      <c r="D58" s="109" t="s">
+        <v>98</v>
+      </c>
+      <c r="E58" s="110"/>
     </row>
     <row r="59" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B59" s="67" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C59" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="D59" s="90" t="s">
-        <v>100</v>
-      </c>
-      <c r="E59" s="91"/>
+        <v>94</v>
+      </c>
+      <c r="D59" s="91" t="s">
+        <v>99</v>
+      </c>
+      <c r="E59" s="93"/>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B13:E16"/>
+    <mergeCell ref="B17:E19"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="D52:E52"/>
@@ -2811,21 +2838,6 @@
     <mergeCell ref="C43:E43"/>
     <mergeCell ref="C44:E44"/>
     <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B13:E16"/>
-    <mergeCell ref="B17:E19"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2840,7 +2852,7 @@
   </sheetPr>
   <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="2" ySplit="14" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
@@ -3365,25 +3377,25 @@
     <row r="15" spans="1:29" s="12" customFormat="1" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25"/>
       <c r="B15" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C15" s="113" t="s">
-        <v>110</v>
-      </c>
-      <c r="D15" s="114"/>
+        <v>123</v>
+      </c>
+      <c r="C15" s="130" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="131"/>
       <c r="K15" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="L15" s="127"/>
-      <c r="M15" s="128"/>
-      <c r="N15" s="127"/>
-      <c r="O15" s="128"/>
-      <c r="P15" s="127"/>
-      <c r="Q15" s="128"/>
-      <c r="R15" s="127"/>
-      <c r="S15" s="128"/>
+      <c r="L15" s="111"/>
+      <c r="M15" s="112"/>
+      <c r="N15" s="111"/>
+      <c r="O15" s="112"/>
+      <c r="P15" s="111"/>
+      <c r="Q15" s="112"/>
+      <c r="R15" s="111"/>
+      <c r="S15" s="112"/>
       <c r="T15" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="U15" s="76"/>
       <c r="V15" s="76"/>
@@ -3398,31 +3410,31 @@
     <row r="16" spans="1:29" s="12" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="111"/>
-      <c r="D16" s="115"/>
-      <c r="E16" s="120" t="s">
-        <v>109</v>
-      </c>
-      <c r="F16" s="121"/>
-      <c r="G16" s="118" t="s">
-        <v>111</v>
-      </c>
-      <c r="H16" s="119"/>
-      <c r="I16" s="129" t="s">
-        <v>119</v>
-      </c>
-      <c r="J16" s="130"/>
+        <v>122</v>
+      </c>
+      <c r="C16" s="117"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="126" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" s="127"/>
+      <c r="G16" s="124" t="s">
+        <v>125</v>
+      </c>
+      <c r="H16" s="125"/>
+      <c r="I16" s="119" t="s">
+        <v>115</v>
+      </c>
+      <c r="J16" s="120"/>
       <c r="K16" s="11"/>
-      <c r="L16" s="125"/>
-      <c r="M16" s="126"/>
-      <c r="N16" s="125"/>
-      <c r="O16" s="126"/>
-      <c r="P16" s="125"/>
-      <c r="Q16" s="126"/>
-      <c r="R16" s="132"/>
-      <c r="S16" s="133"/>
+      <c r="L16" s="115"/>
+      <c r="M16" s="116"/>
+      <c r="N16" s="115"/>
+      <c r="O16" s="116"/>
+      <c r="P16" s="115"/>
+      <c r="Q16" s="116"/>
+      <c r="R16" s="113"/>
+      <c r="S16" s="114"/>
       <c r="T16" s="13"/>
       <c r="U16" s="76"/>
       <c r="V16" s="76"/>
@@ -3437,23 +3449,23 @@
     <row r="17" spans="1:29" s="12" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="23"/>
-      <c r="C17" s="116"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="122"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="112"/>
-      <c r="I17" s="111"/>
-      <c r="J17" s="124"/>
+      <c r="C17" s="121"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="128"/>
+      <c r="F17" s="129"/>
+      <c r="G17" s="117"/>
+      <c r="H17" s="123"/>
+      <c r="I17" s="117"/>
+      <c r="J17" s="118"/>
       <c r="K17" s="11"/>
-      <c r="L17" s="125"/>
-      <c r="M17" s="126"/>
-      <c r="N17" s="125"/>
-      <c r="O17" s="126"/>
-      <c r="P17" s="125"/>
-      <c r="Q17" s="126"/>
-      <c r="R17" s="132"/>
-      <c r="S17" s="133"/>
+      <c r="L17" s="115"/>
+      <c r="M17" s="116"/>
+      <c r="N17" s="115"/>
+      <c r="O17" s="116"/>
+      <c r="P17" s="115"/>
+      <c r="Q17" s="116"/>
+      <c r="R17" s="113"/>
+      <c r="S17" s="114"/>
       <c r="T17" s="13"/>
       <c r="U17" s="76"/>
       <c r="V17" s="76"/>
@@ -3468,23 +3480,23 @@
     <row r="18" spans="1:29" s="12" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="111"/>
-      <c r="H18" s="112"/>
-      <c r="I18" s="116"/>
-      <c r="J18" s="131"/>
+      <c r="C18" s="121"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="123"/>
+      <c r="G18" s="117"/>
+      <c r="H18" s="123"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="122"/>
       <c r="K18" s="11"/>
-      <c r="L18" s="125"/>
-      <c r="M18" s="126"/>
-      <c r="N18" s="125"/>
-      <c r="O18" s="126"/>
-      <c r="P18" s="125"/>
-      <c r="Q18" s="126"/>
-      <c r="R18" s="132"/>
-      <c r="S18" s="133"/>
+      <c r="L18" s="115"/>
+      <c r="M18" s="116"/>
+      <c r="N18" s="115"/>
+      <c r="O18" s="116"/>
+      <c r="P18" s="115"/>
+      <c r="Q18" s="116"/>
+      <c r="R18" s="113"/>
+      <c r="S18" s="114"/>
       <c r="T18" s="13"/>
       <c r="U18" s="76"/>
       <c r="V18" s="76"/>
@@ -3499,23 +3511,23 @@
     <row r="19" spans="1:29" s="12" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="23"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="112"/>
-      <c r="G19" s="111"/>
-      <c r="H19" s="112"/>
-      <c r="I19" s="111"/>
-      <c r="J19" s="124"/>
+      <c r="C19" s="121"/>
+      <c r="D19" s="133"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="123"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="123"/>
+      <c r="I19" s="117"/>
+      <c r="J19" s="118"/>
       <c r="K19" s="11"/>
-      <c r="L19" s="125"/>
-      <c r="M19" s="126"/>
-      <c r="N19" s="125"/>
-      <c r="O19" s="126"/>
-      <c r="P19" s="125"/>
-      <c r="Q19" s="126"/>
-      <c r="R19" s="132"/>
-      <c r="S19" s="133"/>
+      <c r="L19" s="115"/>
+      <c r="M19" s="116"/>
+      <c r="N19" s="115"/>
+      <c r="O19" s="116"/>
+      <c r="P19" s="115"/>
+      <c r="Q19" s="116"/>
+      <c r="R19" s="113"/>
+      <c r="S19" s="114"/>
       <c r="T19" s="13"/>
       <c r="U19" s="76"/>
       <c r="V19" s="76"/>
@@ -3530,23 +3542,23 @@
     <row r="20" spans="1:29" s="12" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="23"/>
-      <c r="C20" s="111"/>
-      <c r="D20" s="112"/>
-      <c r="E20" s="111"/>
-      <c r="F20" s="112"/>
-      <c r="G20" s="111"/>
-      <c r="H20" s="112"/>
-      <c r="I20" s="111"/>
-      <c r="J20" s="124"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="123"/>
+      <c r="G20" s="117"/>
+      <c r="H20" s="123"/>
+      <c r="I20" s="117"/>
+      <c r="J20" s="118"/>
       <c r="K20" s="11"/>
-      <c r="L20" s="125"/>
-      <c r="M20" s="126"/>
-      <c r="N20" s="125"/>
-      <c r="O20" s="126"/>
-      <c r="P20" s="125"/>
-      <c r="Q20" s="126"/>
-      <c r="R20" s="132"/>
-      <c r="S20" s="133"/>
+      <c r="L20" s="115"/>
+      <c r="M20" s="116"/>
+      <c r="N20" s="115"/>
+      <c r="O20" s="116"/>
+      <c r="P20" s="115"/>
+      <c r="Q20" s="116"/>
+      <c r="R20" s="113"/>
+      <c r="S20" s="114"/>
       <c r="T20" s="13"/>
       <c r="U20" s="76"/>
       <c r="V20" s="76"/>
@@ -3561,23 +3573,23 @@
     <row r="21" spans="1:29" s="12" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="23"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="111"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="111"/>
-      <c r="H21" s="112"/>
-      <c r="I21" s="111"/>
-      <c r="J21" s="124"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="123"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="123"/>
+      <c r="G21" s="117"/>
+      <c r="H21" s="123"/>
+      <c r="I21" s="117"/>
+      <c r="J21" s="118"/>
       <c r="K21" s="11"/>
-      <c r="L21" s="125"/>
-      <c r="M21" s="126"/>
-      <c r="N21" s="125"/>
-      <c r="O21" s="126"/>
-      <c r="P21" s="125"/>
-      <c r="Q21" s="126"/>
-      <c r="R21" s="132"/>
-      <c r="S21" s="133"/>
+      <c r="L21" s="115"/>
+      <c r="M21" s="116"/>
+      <c r="N21" s="115"/>
+      <c r="O21" s="116"/>
+      <c r="P21" s="115"/>
+      <c r="Q21" s="116"/>
+      <c r="R21" s="113"/>
+      <c r="S21" s="114"/>
       <c r="T21" s="13"/>
       <c r="U21" s="76"/>
       <c r="V21" s="76"/>
@@ -3591,13 +3603,38 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I19:J19"/>
     <mergeCell ref="P15:Q15"/>
     <mergeCell ref="N21:O21"/>
     <mergeCell ref="N20:O20"/>
@@ -3612,38 +3649,13 @@
     <mergeCell ref="P18:Q18"/>
     <mergeCell ref="P17:Q17"/>
     <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="R16:S16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -3660,7 +3672,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3716,7 +3728,7 @@
     </row>
     <row r="5" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C5" s="39" t="s">
         <v>80</v>
@@ -3732,10 +3744,10 @@
     </row>
     <row r="6" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D6" s="40">
         <v>45575</v>
@@ -3748,17 +3760,17 @@
     </row>
     <row r="7" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D7" s="40">
         <v>45594</v>
       </c>
       <c r="E7" s="41"/>
       <c r="F7" s="39" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G7" s="42">
         <v>0</v>
@@ -3766,7 +3778,7 @@
     </row>
     <row r="8" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C8" s="39" t="s">
         <v>75</v>
@@ -3776,7 +3788,7 @@
       </c>
       <c r="E8" s="41"/>
       <c r="F8" s="39" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G8" s="42">
         <v>0</v>
@@ -5805,7 +5817,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>38</v>
@@ -5928,13 +5940,13 @@
       <c r="A17" s="25"/>
       <c r="B17" s="84"/>
       <c r="C17" s="81" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="82" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" s="82" t="s">
         <v>109</v>
-      </c>
-      <c r="D17" s="82" t="s">
-        <v>124</v>
-      </c>
-      <c r="E17" s="82" t="s">
-        <v>111</v>
       </c>
       <c r="F17" s="83" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
prechod na endoru, novy deadline, upravy/cisteni
</commit_message>
<xml_diff>
--- a/Lean-Projektovy-Management-Prazdna-sablona-JiriBenedikt.com-CZ.xlsx
+++ b/Lean-Projektovy-Management-Prazdna-sablona-JiriBenedikt.com-CZ.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MachacekDav\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KucharJan\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D32308-1B69-486B-89E0-44890CAFA37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD29FF7C-7B76-4203-AD2B-56AEE9B1FDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zakládací listina " sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="134">
   <si>
     <t>Zakládací listina projektu</t>
   </si>
@@ -392,55 +392,61 @@
     <t>Zkrácení času potřebného pro zpracování rezervací oproti tradičním metodám (např. fyzický prodej), s plánem automatizovat 90 % procesů.</t>
   </si>
   <si>
+    <t>výběr a nastavení pluginů</t>
+  </si>
+  <si>
+    <t>Grafický návrh</t>
+  </si>
+  <si>
+    <t>50% Tomáš</t>
+  </si>
+  <si>
+    <t>Registrace na wordpress, vytvoření githubu a násladné pozvání všech členů.</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>Komunikace</t>
+  </si>
+  <si>
+    <t>Začátek a spuštění ENDORY</t>
+  </si>
+  <si>
+    <t>Výběr a instalace Endory platformy</t>
+  </si>
+  <si>
+    <t>instalace Endory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vytvoření webových stránek na platformě Endora. Implementace systému pro online rezervace vstupenek na maturitní ples. Integrace informací o plesu, programu, místě konání a dalších důležitých detailech. </t>
+  </si>
+  <si>
+    <t>Instalace SSL certifikátu, aktualizace Endora a pluginů, použití bezpečnostních pluginů.</t>
+  </si>
+  <si>
+    <t>Výběr platformy Endora</t>
+  </si>
+  <si>
+    <t>Naším cílem je vytvořit webové stránky pomocí platformy Endora, které budou sloužit jako oficiální stránka našeho maturitního plesu. Stránky budou obsahovat možnost online rezervace vstupenek, informace o programu plesu, a další potřebné informace pro účastníky.</t>
+  </si>
+  <si>
     <t>Revize funkčnosti webu a návrhy na úpravy  a testování a příprava na spuštění</t>
   </si>
   <si>
-    <t>výběr a nastavení pluginů</t>
-  </si>
-  <si>
-    <t>Honza kuchař</t>
-  </si>
-  <si>
-    <t>Grafický návrh</t>
-  </si>
-  <si>
-    <t>50% Tomáš</t>
-  </si>
-  <si>
-    <t>Registrace na wordpress, vytvoření githubu a násladné pozvání všech členů.</t>
-  </si>
-  <si>
-    <t>asistent: Filip; nelze</t>
-  </si>
-  <si>
-    <t>SW</t>
-  </si>
-  <si>
-    <t>Komunikace</t>
-  </si>
-  <si>
-    <t>instalace ENDORY</t>
-  </si>
-  <si>
-    <t>Začátek a spuštění ENDORY</t>
-  </si>
-  <si>
-    <t>Výběr a instalace Endory platformy</t>
-  </si>
-  <si>
-    <t>instalace Endory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vytvoření webových stránek na platformě Endora. Implementace systému pro online rezervace vstupenek na maturitní ples. Integrace informací o plesu, programu, místě konání a dalších důležitých detailech. </t>
-  </si>
-  <si>
-    <t>Instalace SSL certifikátu, aktualizace Endora a pluginů, použití bezpečnostních pluginů.</t>
-  </si>
-  <si>
-    <t>Výběr platformy Endora</t>
-  </si>
-  <si>
-    <t>Naším cílem je vytvořit webové stránky pomocí platformy Endora, které budou sloužit jako oficiální stránka našeho maturitního plesu. Stránky budou obsahovat možnost online rezervace vstupenek, informace o programu plesu, a další potřebné informace pro účastníky.</t>
+    <t>Honza Kuchař</t>
+  </si>
+  <si>
+    <t>Navrh databaze na endore</t>
+  </si>
+  <si>
+    <t>nelze</t>
+  </si>
+  <si>
+    <t>20.11.2024</t>
+  </si>
+  <si>
+    <t>asistent: Filip;</t>
   </si>
 </sst>
 </file>
@@ -791,7 +797,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1159,19 +1165,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -1206,6 +1199,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1233,7 +1257,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
@@ -1470,6 +1494,9 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="168" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1537,12 +1564,12 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1558,28 +1585,28 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1593,12 +1620,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1624,6 +1645,24 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="19"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="19" applyFont="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -2319,7 +2358,7 @@
   </sheetPr>
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:E16"/>
     </sheetView>
   </sheetViews>
@@ -2337,13 +2376,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
       <c r="F1" s="64"/>
       <c r="G1" s="64"/>
       <c r="H1" s="64"/>
@@ -2354,28 +2393,28 @@
       <c r="A3" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="107"/>
+      <c r="C3" s="108"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="108" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="107"/>
+      <c r="C4" s="108"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="108" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="107"/>
+      <c r="C5" s="108"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="55" t="s">
@@ -2424,53 +2463,53 @@
       <c r="A13" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="98" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="100"/>
+      <c r="B13" s="99" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="101"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="101"/>
-      <c r="C14" s="102"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="103"/>
+      <c r="B14" s="102"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="104"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="101"/>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="103"/>
+      <c r="B15" s="102"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="103"/>
+      <c r="E15" s="104"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="104"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="106"/>
+      <c r="B16" s="105"/>
+      <c r="C16" s="106"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="107"/>
     </row>
     <row r="17" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="98" t="s">
+      <c r="B17" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="C17" s="99"/>
-      <c r="D17" s="99"/>
-      <c r="E17" s="100"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="101"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="101"/>
-      <c r="C18" s="102"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="103"/>
+      <c r="B18" s="102"/>
+      <c r="C18" s="103"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="104"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="104"/>
-      <c r="C19" s="105"/>
-      <c r="D19" s="105"/>
-      <c r="E19" s="106"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="106"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="107"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="59"/>
@@ -2520,45 +2559,45 @@
       <c r="B26" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="95" t="s">
+      <c r="C26" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="95"/>
-      <c r="E26" s="95"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="96"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="89" t="s">
-        <v>128</v>
-      </c>
-      <c r="C27" s="90" t="s">
+      <c r="B27" s="90" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="90"/>
-      <c r="E27" s="90"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="91"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="89"/>
-      <c r="C28" s="90"/>
-      <c r="D28" s="90"/>
-      <c r="E28" s="90"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="91"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="89"/>
-      <c r="C29" s="90"/>
-      <c r="D29" s="90"/>
-      <c r="E29" s="90"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="91"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="89"/>
-      <c r="C30" s="90"/>
-      <c r="D30" s="90"/>
-      <c r="E30" s="90"/>
+      <c r="B30" s="90"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="91"/>
     </row>
     <row r="31" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="89"/>
-      <c r="C31" s="90"/>
-      <c r="D31" s="90"/>
-      <c r="E31" s="90"/>
+      <c r="B31" s="90"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="91"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="55" t="s">
@@ -2581,7 +2620,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" s="56" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C35" s="63">
         <v>45599</v>
@@ -2618,61 +2657,61 @@
       <c r="B40" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="96" t="s">
+      <c r="C40" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="96"/>
-      <c r="E40" s="96"/>
+      <c r="D40" s="97"/>
+      <c r="E40" s="97"/>
     </row>
     <row r="41" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="91" t="s">
+      <c r="C41" s="92" t="s">
         <v>89</v>
       </c>
-      <c r="D41" s="92"/>
-      <c r="E41" s="93"/>
+      <c r="D41" s="93"/>
+      <c r="E41" s="94"/>
     </row>
     <row r="42" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="91" t="s">
+      <c r="C42" s="92" t="s">
         <v>100</v>
       </c>
-      <c r="D42" s="92"/>
-      <c r="E42" s="93"/>
+      <c r="D42" s="93"/>
+      <c r="E42" s="94"/>
     </row>
     <row r="43" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="91" t="s">
+      <c r="C43" s="92" t="s">
         <v>101</v>
       </c>
-      <c r="D43" s="92"/>
-      <c r="E43" s="93"/>
+      <c r="D43" s="93"/>
+      <c r="E43" s="94"/>
     </row>
     <row r="44" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="C44" s="91" t="s">
+      <c r="C44" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="D44" s="92"/>
-      <c r="E44" s="93"/>
+      <c r="D44" s="93"/>
+      <c r="E44" s="94"/>
     </row>
     <row r="45" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="94" t="s">
-        <v>129</v>
-      </c>
-      <c r="D45" s="94"/>
-      <c r="E45" s="94"/>
+      <c r="C45" s="95" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" s="95"/>
+      <c r="E45" s="95"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="55" t="s">
@@ -2684,25 +2723,25 @@
       <c r="C48" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D48" s="96" t="s">
+      <c r="D48" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="E48" s="96"/>
+      <c r="E48" s="97"/>
     </row>
     <row r="49" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="53" t="s">
         <v>45</v>
       </c>
       <c r="B49" s="65" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C49" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="D49" s="88">
+      <c r="D49" s="89">
         <v>0</v>
       </c>
-      <c r="E49" s="88"/>
+      <c r="E49" s="89"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" s="65" t="s">
@@ -2711,10 +2750,10 @@
       <c r="C50" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="D50" s="88">
+      <c r="D50" s="89">
         <v>0</v>
       </c>
-      <c r="E50" s="88"/>
+      <c r="E50" s="89"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" s="56" t="s">
@@ -2723,10 +2762,10 @@
       <c r="C51" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="D51" s="88">
+      <c r="D51" s="89">
         <v>0</v>
       </c>
-      <c r="E51" s="88"/>
+      <c r="E51" s="89"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="56" t="s">
@@ -2735,10 +2774,10 @@
       <c r="C52" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="D52" s="88">
+      <c r="D52" s="89">
         <v>0</v>
       </c>
-      <c r="E52" s="88"/>
+      <c r="E52" s="89"/>
     </row>
     <row r="53" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B53" s="56" t="s">
@@ -2747,16 +2786,16 @@
       <c r="C53" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="D53" s="88">
+      <c r="D53" s="89">
         <v>0</v>
       </c>
-      <c r="E53" s="88"/>
+      <c r="E53" s="89"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" s="69"/>
       <c r="C54" s="69"/>
-      <c r="D54" s="108"/>
-      <c r="E54" s="108"/>
+      <c r="D54" s="109"/>
+      <c r="E54" s="109"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="55" t="s">
@@ -2779,10 +2818,10 @@
       <c r="C57" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="D57" s="91" t="s">
+      <c r="D57" s="92" t="s">
         <v>95</v>
       </c>
-      <c r="E57" s="93"/>
+      <c r="E57" s="94"/>
     </row>
     <row r="58" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B58" s="67" t="s">
@@ -2791,10 +2830,10 @@
       <c r="C58" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="D58" s="109" t="s">
+      <c r="D58" s="110" t="s">
         <v>98</v>
       </c>
-      <c r="E58" s="110"/>
+      <c r="E58" s="111"/>
     </row>
     <row r="59" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B59" s="67" t="s">
@@ -2803,10 +2842,10 @@
       <c r="C59" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="D59" s="91" t="s">
+      <c r="D59" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="E59" s="93"/>
+      <c r="E59" s="94"/>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70"/>
@@ -2852,11 +2891,11 @@
   </sheetPr>
   <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="14" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="14" topLeftCell="J15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16:J16"/>
+      <selection pane="bottomRight" activeCell="P18" sqref="P18:Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2982,67 +3021,74 @@
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B4" s="2"/>
       <c r="C4" s="5">
+        <v>45552</v>
+      </c>
+      <c r="D4" s="5">
+        <f>C4+7</f>
         <v>45559</v>
       </c>
-      <c r="D4" s="5">
+      <c r="E4" s="5">
+        <f t="shared" ref="E4:J4" si="0">D4+7</f>
         <v>45566</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
+        <f t="shared" si="0"/>
         <v>45573</v>
       </c>
-      <c r="F4" s="5">
+      <c r="G4" s="5">
+        <f t="shared" si="0"/>
         <v>45580</v>
       </c>
-      <c r="G4" s="5">
+      <c r="H4" s="5">
+        <f t="shared" si="0"/>
         <v>45587</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
+        <f t="shared" si="0"/>
         <v>45594</v>
       </c>
-      <c r="I4" s="5">
+      <c r="J4" s="5">
+        <f t="shared" si="0"/>
         <v>45601</v>
       </c>
-      <c r="J4" s="5">
+      <c r="K4" s="6">
         <v>45608</v>
-      </c>
-      <c r="K4" s="6">
-        <v>45615</v>
       </c>
       <c r="L4" s="5">
         <f>K4+7</f>
-        <v>45622</v>
+        <v>45615</v>
       </c>
       <c r="M4" s="5">
         <f>L4+7</f>
+        <v>45622</v>
+      </c>
+      <c r="N4" s="5">
+        <f t="shared" ref="N4:S4" si="1">M4+7</f>
         <v>45629</v>
       </c>
-      <c r="N4" s="5">
-        <f t="shared" ref="N4:S4" si="0">M4+7</f>
+      <c r="O4" s="5">
+        <f t="shared" si="1"/>
         <v>45636</v>
       </c>
-      <c r="O4" s="5">
-        <f t="shared" si="0"/>
+      <c r="P4" s="5">
+        <f t="shared" si="1"/>
         <v>45643</v>
       </c>
-      <c r="P4" s="5">
-        <f t="shared" si="0"/>
+      <c r="Q4" s="5">
+        <f t="shared" si="1"/>
         <v>45650</v>
       </c>
-      <c r="Q4" s="5">
-        <f t="shared" si="0"/>
+      <c r="R4" s="5">
+        <f t="shared" si="1"/>
         <v>45657</v>
       </c>
-      <c r="R4" s="5">
-        <f t="shared" si="0"/>
+      <c r="S4" s="5">
+        <f t="shared" si="1"/>
         <v>45664</v>
-      </c>
-      <c r="S4" s="5">
-        <f t="shared" si="0"/>
-        <v>45671</v>
       </c>
       <c r="T4" s="6">
         <f>S4+6</f>
-        <v>45677</v>
+        <v>45670</v>
       </c>
       <c r="U4" s="72"/>
       <c r="V4" s="72"/>
@@ -3377,23 +3423,23 @@
     <row r="15" spans="1:29" s="12" customFormat="1" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25"/>
       <c r="B15" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" s="130" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="125" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="131"/>
-      <c r="K15" s="11" t="s">
+      <c r="D15" s="126"/>
+      <c r="K15" s="88" t="s">
         <v>84</v>
       </c>
-      <c r="L15" s="111"/>
-      <c r="M15" s="112"/>
-      <c r="N15" s="111"/>
-      <c r="O15" s="112"/>
-      <c r="P15" s="111"/>
-      <c r="Q15" s="112"/>
-      <c r="R15" s="111"/>
-      <c r="S15" s="112"/>
+      <c r="L15" s="112"/>
+      <c r="M15" s="113"/>
+      <c r="N15" s="112"/>
+      <c r="O15" s="113"/>
+      <c r="P15" s="112"/>
+      <c r="Q15" s="113"/>
+      <c r="R15" s="112"/>
+      <c r="S15" s="113"/>
       <c r="T15" s="13" t="s">
         <v>105</v>
       </c>
@@ -3410,31 +3456,35 @@
     <row r="16" spans="1:29" s="12" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="C16" s="117"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="126" t="s">
-        <v>124</v>
-      </c>
-      <c r="F16" s="127"/>
-      <c r="G16" s="124" t="s">
-        <v>125</v>
-      </c>
-      <c r="H16" s="125"/>
-      <c r="I16" s="119" t="s">
-        <v>115</v>
-      </c>
-      <c r="J16" s="120"/>
+        <v>119</v>
+      </c>
+      <c r="C16" s="118"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="127" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="128"/>
+      <c r="G16" s="140" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="141"/>
+      <c r="I16" s="141" t="s">
+        <v>128</v>
+      </c>
+      <c r="J16" s="142"/>
       <c r="K16" s="11"/>
-      <c r="L16" s="115"/>
-      <c r="M16" s="116"/>
-      <c r="N16" s="115"/>
-      <c r="O16" s="116"/>
-      <c r="P16" s="115"/>
-      <c r="Q16" s="116"/>
-      <c r="R16" s="113"/>
-      <c r="S16" s="114"/>
+      <c r="L16" s="125" t="s">
+        <v>121</v>
+      </c>
+      <c r="M16" s="126"/>
+      <c r="N16" s="120"/>
+      <c r="O16" s="121"/>
+      <c r="P16" s="116"/>
+      <c r="Q16" s="117"/>
+      <c r="R16" s="143" t="s">
+        <v>128</v>
+      </c>
+      <c r="S16" s="144"/>
       <c r="T16" s="13"/>
       <c r="U16" s="76"/>
       <c r="V16" s="76"/>
@@ -3449,23 +3499,23 @@
     <row r="17" spans="1:29" s="12" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="23"/>
-      <c r="C17" s="121"/>
-      <c r="D17" s="133"/>
-      <c r="E17" s="128"/>
-      <c r="F17" s="129"/>
-      <c r="G17" s="117"/>
-      <c r="H17" s="123"/>
-      <c r="I17" s="117"/>
-      <c r="J17" s="118"/>
+      <c r="C17" s="122"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="129"/>
+      <c r="F17" s="130"/>
+      <c r="G17" s="118"/>
+      <c r="H17" s="124"/>
+      <c r="I17" s="118"/>
+      <c r="J17" s="119"/>
       <c r="K17" s="11"/>
-      <c r="L17" s="115"/>
-      <c r="M17" s="116"/>
-      <c r="N17" s="115"/>
-      <c r="O17" s="116"/>
-      <c r="P17" s="115"/>
-      <c r="Q17" s="116"/>
-      <c r="R17" s="113"/>
-      <c r="S17" s="114"/>
+      <c r="L17" s="116"/>
+      <c r="M17" s="117"/>
+      <c r="N17" s="116"/>
+      <c r="O17" s="117"/>
+      <c r="P17" s="116"/>
+      <c r="Q17" s="117"/>
+      <c r="R17" s="114"/>
+      <c r="S17" s="115"/>
       <c r="T17" s="13"/>
       <c r="U17" s="76"/>
       <c r="V17" s="76"/>
@@ -3480,23 +3530,23 @@
     <row r="18" spans="1:29" s="12" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="121"/>
-      <c r="D18" s="133"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="123"/>
-      <c r="G18" s="117"/>
-      <c r="H18" s="123"/>
-      <c r="I18" s="121"/>
-      <c r="J18" s="122"/>
+      <c r="C18" s="122"/>
+      <c r="D18" s="132"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="124"/>
+      <c r="I18" s="122"/>
+      <c r="J18" s="123"/>
       <c r="K18" s="11"/>
-      <c r="L18" s="115"/>
-      <c r="M18" s="116"/>
-      <c r="N18" s="115"/>
-      <c r="O18" s="116"/>
-      <c r="P18" s="115"/>
-      <c r="Q18" s="116"/>
-      <c r="R18" s="113"/>
-      <c r="S18" s="114"/>
+      <c r="L18" s="116"/>
+      <c r="M18" s="117"/>
+      <c r="N18" s="116"/>
+      <c r="O18" s="117"/>
+      <c r="P18" s="116"/>
+      <c r="Q18" s="117"/>
+      <c r="R18" s="114"/>
+      <c r="S18" s="115"/>
       <c r="T18" s="13"/>
       <c r="U18" s="76"/>
       <c r="V18" s="76"/>
@@ -3511,23 +3561,23 @@
     <row r="19" spans="1:29" s="12" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="23"/>
-      <c r="C19" s="121"/>
-      <c r="D19" s="133"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="117"/>
-      <c r="H19" s="123"/>
-      <c r="I19" s="117"/>
-      <c r="J19" s="118"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="118"/>
+      <c r="H19" s="124"/>
+      <c r="I19" s="118"/>
+      <c r="J19" s="119"/>
       <c r="K19" s="11"/>
-      <c r="L19" s="115"/>
-      <c r="M19" s="116"/>
-      <c r="N19" s="115"/>
-      <c r="O19" s="116"/>
-      <c r="P19" s="115"/>
-      <c r="Q19" s="116"/>
-      <c r="R19" s="113"/>
-      <c r="S19" s="114"/>
+      <c r="L19" s="116"/>
+      <c r="M19" s="117"/>
+      <c r="N19" s="116"/>
+      <c r="O19" s="117"/>
+      <c r="P19" s="116"/>
+      <c r="Q19" s="117"/>
+      <c r="R19" s="114"/>
+      <c r="S19" s="115"/>
       <c r="T19" s="13"/>
       <c r="U19" s="76"/>
       <c r="V19" s="76"/>
@@ -3542,23 +3592,23 @@
     <row r="20" spans="1:29" s="12" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="23"/>
-      <c r="C20" s="117"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="117"/>
-      <c r="F20" s="123"/>
-      <c r="G20" s="117"/>
-      <c r="H20" s="123"/>
-      <c r="I20" s="117"/>
-      <c r="J20" s="118"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="124"/>
+      <c r="E20" s="118"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="118"/>
+      <c r="H20" s="124"/>
+      <c r="I20" s="118"/>
+      <c r="J20" s="119"/>
       <c r="K20" s="11"/>
-      <c r="L20" s="115"/>
-      <c r="M20" s="116"/>
-      <c r="N20" s="115"/>
-      <c r="O20" s="116"/>
-      <c r="P20" s="115"/>
-      <c r="Q20" s="116"/>
-      <c r="R20" s="113"/>
-      <c r="S20" s="114"/>
+      <c r="L20" s="116"/>
+      <c r="M20" s="117"/>
+      <c r="N20" s="116"/>
+      <c r="O20" s="117"/>
+      <c r="P20" s="116"/>
+      <c r="Q20" s="117"/>
+      <c r="R20" s="114"/>
+      <c r="S20" s="115"/>
       <c r="T20" s="13"/>
       <c r="U20" s="76"/>
       <c r="V20" s="76"/>
@@ -3573,23 +3623,23 @@
     <row r="21" spans="1:29" s="12" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="23"/>
-      <c r="C21" s="117"/>
-      <c r="D21" s="123"/>
-      <c r="E21" s="117"/>
-      <c r="F21" s="123"/>
-      <c r="G21" s="117"/>
-      <c r="H21" s="123"/>
-      <c r="I21" s="117"/>
-      <c r="J21" s="118"/>
+      <c r="C21" s="118"/>
+      <c r="D21" s="124"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="118"/>
+      <c r="H21" s="124"/>
+      <c r="I21" s="118"/>
+      <c r="J21" s="119"/>
       <c r="K21" s="11"/>
-      <c r="L21" s="115"/>
-      <c r="M21" s="116"/>
-      <c r="N21" s="115"/>
-      <c r="O21" s="116"/>
-      <c r="P21" s="115"/>
-      <c r="Q21" s="116"/>
-      <c r="R21" s="113"/>
-      <c r="S21" s="114"/>
+      <c r="L21" s="116"/>
+      <c r="M21" s="117"/>
+      <c r="N21" s="116"/>
+      <c r="O21" s="117"/>
+      <c r="P21" s="116"/>
+      <c r="Q21" s="117"/>
+      <c r="R21" s="114"/>
+      <c r="S21" s="115"/>
       <c r="T21" s="13"/>
       <c r="U21" s="76"/>
       <c r="V21" s="76"/>
@@ -3611,7 +3661,7 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="L16:M16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G19:H19"/>
@@ -3622,15 +3672,15 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G16:H16"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L16:M16"/>
     <mergeCell ref="L21:M21"/>
     <mergeCell ref="L20:M20"/>
     <mergeCell ref="L19:M19"/>
     <mergeCell ref="L18:M18"/>
-    <mergeCell ref="I16:J16"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="I20:J20"/>
@@ -3641,7 +3691,6 @@
     <mergeCell ref="N19:O19"/>
     <mergeCell ref="N18:O18"/>
     <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N16:O16"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="P21:Q21"/>
     <mergeCell ref="P20:Q20"/>
@@ -3649,6 +3698,7 @@
     <mergeCell ref="P18:Q18"/>
     <mergeCell ref="P17:Q17"/>
     <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="N16:O16"/>
     <mergeCell ref="R15:S15"/>
     <mergeCell ref="R21:S21"/>
     <mergeCell ref="R20:S20"/>
@@ -3672,7 +3722,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3690,21 +3740,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="133" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="133"/>
     </row>
     <row r="3" spans="2:7" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="134"/>
       <c r="E3" s="34"/>
-      <c r="F3" s="136"/>
-      <c r="G3" s="136"/>
+      <c r="F3" s="135"/>
+      <c r="G3" s="135"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
@@ -3744,7 +3794,7 @@
     </row>
     <row r="6" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C6" s="39" t="s">
         <v>110</v>
@@ -3760,17 +3810,19 @@
     </row>
     <row r="7" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D7" s="40">
         <v>45594</v>
       </c>
-      <c r="E7" s="41"/>
+      <c r="E7" s="41" t="s">
+        <v>131</v>
+      </c>
       <c r="F7" s="39" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="G7" s="42">
         <v>0</v>
@@ -3778,7 +3830,7 @@
     </row>
     <row r="8" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C8" s="39" t="s">
         <v>75</v>
@@ -3786,21 +3838,31 @@
       <c r="D8" s="40">
         <v>45594</v>
       </c>
-      <c r="E8" s="41"/>
+      <c r="E8" s="145" t="s">
+        <v>132</v>
+      </c>
       <c r="F8" s="39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G8" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="38"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="40">
+        <v>45603</v>
+      </c>
       <c r="E9" s="40"/>
       <c r="F9" s="39"/>
-      <c r="G9" s="42"/>
+      <c r="G9" s="42">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="38"/>
@@ -5804,13 +5866,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="136" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
     </row>
     <row r="4" spans="2:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
@@ -5943,7 +6005,7 @@
         <v>107</v>
       </c>
       <c r="D17" s="82" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E17" s="82" t="s">
         <v>109</v>
@@ -6049,13 +6111,13 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="138" t="s">
+      <c r="B7" s="137" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="138"/>
-      <c r="D7" s="138"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="138"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="31"/>
@@ -6087,18 +6149,18 @@
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="139" t="s">
+      <c r="D13" s="138" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="139"/>
+      <c r="E13" s="138"/>
       <c r="F13" s="30"/>
       <c r="H13" s="30"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="140" t="s">
+      <c r="D14" s="139" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="140"/>
+      <c r="E14" s="139"/>
       <c r="F14" s="30"/>
       <c r="G14" s="30"/>
       <c r="H14" s="30"/>

</xml_diff>